<commit_message>
full functionality; spreadsheet and script complete
</commit_message>
<xml_diff>
--- a/Champion-Runes.xlsx
+++ b/Champion-Runes.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Duc\Desktop\IRL Useful\ARAM Runes Assistant\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{878563CF-CC14-462D-8D76-B50B42833F37}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DE0D3D3-8B28-480C-8CBA-374ACA357A73}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20115" yWindow="345" windowWidth="3960" windowHeight="8685" tabRatio="646" firstSheet="4" activeTab="4" xr2:uid="{05130611-41D6-43C8-B73A-9762CE92870A}"/>
-    <workbookView xWindow="-24540" yWindow="2085" windowWidth="28800" windowHeight="7830" xr2:uid="{0F249C26-87E6-4EFF-B5DE-0EE0792CAA0B}"/>
-    <workbookView xWindow="24420" yWindow="8175" windowWidth="3480" windowHeight="7830" firstSheet="6" activeTab="6" xr2:uid="{B0B8A4CF-9A6F-48B0-AD68-9ED65BEAE22B}"/>
-    <workbookView xWindow="24210" yWindow="525" windowWidth="4455" windowHeight="8670" firstSheet="2" activeTab="2" xr2:uid="{FF81866E-A5AA-4548-837C-48FE481E8A96}"/>
-    <workbookView xWindow="15855" yWindow="360" windowWidth="3735" windowHeight="7830" firstSheet="5" activeTab="5" xr2:uid="{3EC68EC8-DD93-4836-B4ED-D69B4814133D}"/>
-    <workbookView xWindow="16050" yWindow="7665" windowWidth="4395" windowHeight="8670" firstSheet="1" activeTab="1" xr2:uid="{E34CFB41-02AE-4BB4-960D-A9D095459DFB}"/>
-    <workbookView xWindow="20685" yWindow="8070" windowWidth="3675" windowHeight="7830" activeTab="3" xr2:uid="{01F08989-AD10-4245-9BC1-75968EBDD16D}"/>
+    <workbookView xWindow="20775" yWindow="30" windowWidth="3690" windowHeight="8370" tabRatio="646" firstSheet="4" activeTab="4" xr2:uid="{05130611-41D6-43C8-B73A-9762CE92870A}"/>
+    <workbookView xWindow="0" yWindow="7800" windowWidth="9600" windowHeight="7800" xr2:uid="{0F249C26-87E6-4EFF-B5DE-0EE0792CAA0B}"/>
+    <workbookView xWindow="17130" yWindow="7785" windowWidth="3300" windowHeight="6435" firstSheet="6" activeTab="6" xr2:uid="{B0B8A4CF-9A6F-48B0-AD68-9ED65BEAE22B}"/>
+    <workbookView xWindow="24435" yWindow="30" windowWidth="4410" windowHeight="8205" firstSheet="2" activeTab="2" xr2:uid="{FF81866E-A5AA-4548-837C-48FE481E8A96}"/>
+    <workbookView xWindow="25065" yWindow="7515" windowWidth="3705" windowHeight="8220" firstSheet="5" activeTab="5" xr2:uid="{3EC68EC8-DD93-4836-B4ED-D69B4814133D}"/>
+    <workbookView xWindow="20610" yWindow="7620" windowWidth="4350" windowHeight="8175" firstSheet="1" activeTab="1" xr2:uid="{E34CFB41-02AE-4BB4-960D-A9D095459DFB}"/>
+    <workbookView xWindow="17055" yWindow="30" windowWidth="3690" windowHeight="8055" activeTab="3" xr2:uid="{01F08989-AD10-4245-9BC1-75968EBDD16D}"/>
   </bookViews>
   <sheets>
     <sheet name="Champion Runes" sheetId="1" r:id="rId1"/>
@@ -28,6 +28,7 @@
     <sheet name="Stats" sheetId="17" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="166">
   <si>
     <t>Keystone</t>
   </si>
@@ -513,34 +514,34 @@
     <t>Inspiration</t>
   </si>
   <si>
-    <t>Kai'Sa (AP)</t>
-  </si>
-  <si>
-    <t>Kai'Sa (AD)</t>
-  </si>
-  <si>
-    <t>Malphite (AP)</t>
-  </si>
-  <si>
-    <t>Malphite (TANK)</t>
-  </si>
-  <si>
-    <t>Miss Fortune (AP)</t>
-  </si>
-  <si>
-    <t>Miss Fortune (AD)</t>
-  </si>
-  <si>
     <t>Nocturne</t>
   </si>
   <si>
-    <t>Varus (POKE)</t>
-  </si>
-  <si>
-    <t>Varus (ONHIT)</t>
-  </si>
-  <si>
     <t>Champion Name</t>
+  </si>
+  <si>
+    <t>Varus ONHIT</t>
+  </si>
+  <si>
+    <t>Varus POKE</t>
+  </si>
+  <si>
+    <t>Miss Fortune AP</t>
+  </si>
+  <si>
+    <t>Miss Fortune AD</t>
+  </si>
+  <si>
+    <t>Malphite AP</t>
+  </si>
+  <si>
+    <t>Malphite TANK</t>
+  </si>
+  <si>
+    <t>Kai'Sa AP</t>
+  </si>
+  <si>
+    <t>Kai'Sa AD</t>
   </si>
 </sst>
 </file>
@@ -1953,8 +1954,8 @@
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H22" sqref="H22"/>
     </sheetView>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="1">
-      <selection activeCell="G87" sqref="G87"/>
+    <sheetView tabSelected="1" workbookViewId="1">
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
     <sheetView workbookViewId="2"/>
     <sheetView workbookViewId="3"/>
@@ -1975,7 +1976,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>145</v>
@@ -3799,7 +3800,7 @@
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>144</v>
@@ -3837,7 +3838,7 @@
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>146</v>
@@ -4597,7 +4598,7 @@
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>147</v>
@@ -4635,7 +4636,7 @@
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>146</v>
@@ -5129,13 +5130,40 @@
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="B84" s="2" t="s">
         <v>146</v>
       </c>
+      <c r="C84" s="2">
+        <v>6</v>
+      </c>
+      <c r="D84" s="2">
+        <v>29</v>
+      </c>
       <c r="E84" s="2">
         <v>27</v>
+      </c>
+      <c r="F84" s="2">
+        <v>31</v>
+      </c>
+      <c r="G84" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="H84" s="2">
+        <v>17</v>
+      </c>
+      <c r="I84" s="2">
+        <v>22</v>
+      </c>
+      <c r="J84" s="2">
+        <v>1</v>
+      </c>
+      <c r="K84" s="2">
+        <v>1</v>
+      </c>
+      <c r="L84" s="2">
+        <v>6</v>
       </c>
     </row>
     <row r="85" spans="1:12" x14ac:dyDescent="0.25">
@@ -5145,6 +5173,36 @@
       <c r="B85" s="2" t="s">
         <v>147</v>
       </c>
+      <c r="C85" s="2">
+        <v>12</v>
+      </c>
+      <c r="D85" s="2">
+        <v>45</v>
+      </c>
+      <c r="E85" s="2">
+        <v>48</v>
+      </c>
+      <c r="F85" s="2">
+        <v>49</v>
+      </c>
+      <c r="G85" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="H85" s="2">
+        <v>17</v>
+      </c>
+      <c r="I85" s="2">
+        <v>20</v>
+      </c>
+      <c r="J85" s="2">
+        <v>1</v>
+      </c>
+      <c r="K85" s="2">
+        <v>4</v>
+      </c>
+      <c r="L85" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="86" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
@@ -5153,6 +5211,36 @@
       <c r="B86" s="2" t="s">
         <v>144</v>
       </c>
+      <c r="C86" s="2">
+        <v>69</v>
+      </c>
+      <c r="D86" s="2">
+        <v>17</v>
+      </c>
+      <c r="E86" s="2">
+        <v>21</v>
+      </c>
+      <c r="F86" s="2">
+        <v>24</v>
+      </c>
+      <c r="G86" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="H86" s="2">
+        <v>50</v>
+      </c>
+      <c r="I86" s="2">
+        <v>51</v>
+      </c>
+      <c r="J86" s="2">
+        <v>2</v>
+      </c>
+      <c r="K86" s="2">
+        <v>1</v>
+      </c>
+      <c r="L86" s="2">
+        <v>6</v>
+      </c>
     </row>
     <row r="87" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
@@ -5161,6 +5249,36 @@
       <c r="B87" s="2" t="s">
         <v>148</v>
       </c>
+      <c r="C87" s="2">
+        <v>7</v>
+      </c>
+      <c r="D87" s="2">
+        <v>35</v>
+      </c>
+      <c r="E87" s="2">
+        <v>37</v>
+      </c>
+      <c r="F87" s="2">
+        <v>40</v>
+      </c>
+      <c r="G87" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="H87" s="2">
+        <v>18</v>
+      </c>
+      <c r="I87" s="2">
+        <v>22</v>
+      </c>
+      <c r="J87" s="2">
+        <v>1</v>
+      </c>
+      <c r="K87" s="2">
+        <v>1</v>
+      </c>
+      <c r="L87" s="2">
+        <v>6</v>
+      </c>
     </row>
     <row r="88" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
@@ -5169,6 +5287,36 @@
       <c r="B88" s="2" t="s">
         <v>147</v>
       </c>
+      <c r="C88" s="2">
+        <v>10</v>
+      </c>
+      <c r="D88" s="2">
+        <v>73</v>
+      </c>
+      <c r="E88" s="2">
+        <v>48</v>
+      </c>
+      <c r="F88" s="2">
+        <v>49</v>
+      </c>
+      <c r="G88" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="H88" s="2">
+        <v>17</v>
+      </c>
+      <c r="I88" s="2">
+        <v>20</v>
+      </c>
+      <c r="J88" s="2">
+        <v>1</v>
+      </c>
+      <c r="K88" s="2">
+        <v>4</v>
+      </c>
+      <c r="L88" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="89" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
@@ -5177,6 +5325,36 @@
       <c r="B89" s="2" t="s">
         <v>144</v>
       </c>
+      <c r="C89" s="2">
+        <v>69</v>
+      </c>
+      <c r="D89" s="2">
+        <v>17</v>
+      </c>
+      <c r="E89" s="2">
+        <v>20</v>
+      </c>
+      <c r="F89" s="2">
+        <v>22</v>
+      </c>
+      <c r="G89" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="H89" s="2">
+        <v>50</v>
+      </c>
+      <c r="I89" s="2">
+        <v>66</v>
+      </c>
+      <c r="J89" s="2">
+        <v>1</v>
+      </c>
+      <c r="K89" s="2">
+        <v>4</v>
+      </c>
+      <c r="L89" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="90" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
@@ -5185,6 +5363,36 @@
       <c r="B90" s="2" t="s">
         <v>147</v>
       </c>
+      <c r="C90" s="2">
+        <v>12</v>
+      </c>
+      <c r="D90" s="2">
+        <v>45</v>
+      </c>
+      <c r="E90" s="2">
+        <v>48</v>
+      </c>
+      <c r="F90" s="2">
+        <v>49</v>
+      </c>
+      <c r="G90" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="H90" s="2">
+        <v>17</v>
+      </c>
+      <c r="I90" s="2">
+        <v>20</v>
+      </c>
+      <c r="J90" s="2">
+        <v>1</v>
+      </c>
+      <c r="K90" s="2">
+        <v>4</v>
+      </c>
+      <c r="L90" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="91" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
@@ -5193,6 +5401,36 @@
       <c r="B91" s="2" t="s">
         <v>147</v>
       </c>
+      <c r="C91" s="2">
+        <v>12</v>
+      </c>
+      <c r="D91" s="2">
+        <v>45</v>
+      </c>
+      <c r="E91" s="2">
+        <v>66</v>
+      </c>
+      <c r="F91" s="2">
+        <v>50</v>
+      </c>
+      <c r="G91" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="H91" s="2">
+        <v>30</v>
+      </c>
+      <c r="I91" s="2">
+        <v>72</v>
+      </c>
+      <c r="J91" s="2">
+        <v>1</v>
+      </c>
+      <c r="K91" s="2">
+        <v>4</v>
+      </c>
+      <c r="L91" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="92" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
@@ -5201,8 +5439,35 @@
       <c r="B92" s="2" t="s">
         <v>146</v>
       </c>
+      <c r="C92" s="2">
+        <v>6</v>
+      </c>
+      <c r="D92" s="2">
+        <v>30</v>
+      </c>
       <c r="E92" s="2">
         <v>27</v>
+      </c>
+      <c r="F92" s="2">
+        <v>31</v>
+      </c>
+      <c r="G92" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="H92" s="2">
+        <v>17</v>
+      </c>
+      <c r="I92" s="2">
+        <v>22</v>
+      </c>
+      <c r="J92" s="2">
+        <v>1</v>
+      </c>
+      <c r="K92" s="2">
+        <v>1</v>
+      </c>
+      <c r="L92" s="2">
+        <v>6</v>
       </c>
     </row>
     <row r="93" spans="1:12" x14ac:dyDescent="0.25">
@@ -5212,6 +5477,36 @@
       <c r="B93" s="2" t="s">
         <v>144</v>
       </c>
+      <c r="C93" s="2">
+        <v>1</v>
+      </c>
+      <c r="D93" s="2">
+        <v>17</v>
+      </c>
+      <c r="E93" s="2">
+        <v>21</v>
+      </c>
+      <c r="F93" s="2">
+        <v>22</v>
+      </c>
+      <c r="G93" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="H93" s="2">
+        <v>29</v>
+      </c>
+      <c r="I93" s="2">
+        <v>27</v>
+      </c>
+      <c r="J93" s="2">
+        <v>2</v>
+      </c>
+      <c r="K93" s="2">
+        <v>1</v>
+      </c>
+      <c r="L93" s="2">
+        <v>6</v>
+      </c>
     </row>
     <row r="94" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
@@ -5220,6 +5515,36 @@
       <c r="B94" s="2" t="s">
         <v>147</v>
       </c>
+      <c r="C94" s="2">
+        <v>12</v>
+      </c>
+      <c r="D94" s="2">
+        <v>45</v>
+      </c>
+      <c r="E94" s="2">
+        <v>66</v>
+      </c>
+      <c r="F94" s="2">
+        <v>50</v>
+      </c>
+      <c r="G94" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="H94" s="2">
+        <v>70</v>
+      </c>
+      <c r="I94" s="2">
+        <v>38</v>
+      </c>
+      <c r="J94" s="2">
+        <v>3</v>
+      </c>
+      <c r="K94" s="2">
+        <v>4</v>
+      </c>
+      <c r="L94" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="95" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
@@ -5228,6 +5553,36 @@
       <c r="B95" s="2" t="s">
         <v>147</v>
       </c>
+      <c r="C95" s="2">
+        <v>12</v>
+      </c>
+      <c r="D95" s="2">
+        <v>44</v>
+      </c>
+      <c r="E95" s="2">
+        <v>48</v>
+      </c>
+      <c r="F95" s="2">
+        <v>49</v>
+      </c>
+      <c r="G95" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="H95" s="2">
+        <v>17</v>
+      </c>
+      <c r="I95" s="2">
+        <v>20</v>
+      </c>
+      <c r="J95" s="2">
+        <v>1</v>
+      </c>
+      <c r="K95" s="2">
+        <v>4</v>
+      </c>
+      <c r="L95" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="96" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
@@ -5236,506 +5591,2087 @@
       <c r="B96" s="2" t="s">
         <v>146</v>
       </c>
+      <c r="C96" s="2">
+        <v>71</v>
+      </c>
+      <c r="D96" s="2">
+        <v>28</v>
+      </c>
       <c r="E96" s="2">
         <v>27</v>
       </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F96" s="2">
+        <v>31</v>
+      </c>
+      <c r="G96" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="H96" s="2">
+        <v>17</v>
+      </c>
+      <c r="I96" s="2">
+        <v>22</v>
+      </c>
+      <c r="J96" s="2">
+        <v>1</v>
+      </c>
+      <c r="K96" s="2">
+        <v>1</v>
+      </c>
+      <c r="L96" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>92</v>
       </c>
       <c r="B97" s="2" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C97" s="2">
+        <v>69</v>
+      </c>
+      <c r="D97" s="2">
+        <v>17</v>
+      </c>
+      <c r="E97" s="2">
+        <v>20</v>
+      </c>
+      <c r="F97" s="2">
+        <v>22</v>
+      </c>
+      <c r="G97" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="H97" s="2">
+        <v>31</v>
+      </c>
+      <c r="I97" s="2">
+        <v>30</v>
+      </c>
+      <c r="J97" s="2">
+        <v>1</v>
+      </c>
+      <c r="K97" s="2">
+        <v>1</v>
+      </c>
+      <c r="L97" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>93</v>
       </c>
       <c r="B98" s="2" t="s">
         <v>146</v>
       </c>
+      <c r="C98" s="2">
+        <v>6</v>
+      </c>
+      <c r="D98" s="2">
+        <v>30</v>
+      </c>
       <c r="E98" s="2">
         <v>27</v>
       </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F98" s="2">
+        <v>31</v>
+      </c>
+      <c r="G98" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="H98" s="2">
+        <v>17</v>
+      </c>
+      <c r="I98" s="2">
+        <v>22</v>
+      </c>
+      <c r="J98" s="2">
+        <v>1</v>
+      </c>
+      <c r="K98" s="2">
+        <v>1</v>
+      </c>
+      <c r="L98" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>94</v>
       </c>
       <c r="B99" s="2" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C99" s="2">
+        <v>69</v>
+      </c>
+      <c r="D99" s="2">
+        <v>17</v>
+      </c>
+      <c r="E99" s="2">
+        <v>20</v>
+      </c>
+      <c r="F99" s="2">
+        <v>22</v>
+      </c>
+      <c r="G99" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="H99" s="2">
+        <v>31</v>
+      </c>
+      <c r="I99" s="2">
+        <v>30</v>
+      </c>
+      <c r="J99" s="2">
+        <v>1</v>
+      </c>
+      <c r="K99" s="2">
+        <v>4</v>
+      </c>
+      <c r="L99" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>95</v>
       </c>
       <c r="B100" s="2" t="s">
         <v>146</v>
       </c>
+      <c r="C100" s="2">
+        <v>6</v>
+      </c>
+      <c r="D100" s="2">
+        <v>29</v>
+      </c>
       <c r="E100" s="2">
         <v>27</v>
       </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F100" s="2">
+        <v>72</v>
+      </c>
+      <c r="G100" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="H100" s="2">
+        <v>18</v>
+      </c>
+      <c r="I100" s="2">
+        <v>22</v>
+      </c>
+      <c r="J100" s="2">
+        <v>1</v>
+      </c>
+      <c r="K100" s="2">
+        <v>1</v>
+      </c>
+      <c r="L100" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>96</v>
       </c>
       <c r="B101" s="2" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C101" s="2">
+        <v>9</v>
+      </c>
+      <c r="D101" s="2">
+        <v>35</v>
+      </c>
+      <c r="E101" s="2">
+        <v>37</v>
+      </c>
+      <c r="F101" s="2">
+        <v>40</v>
+      </c>
+      <c r="G101" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="H101" s="2">
+        <v>18</v>
+      </c>
+      <c r="I101" s="2">
+        <v>22</v>
+      </c>
+      <c r="J101" s="2">
+        <v>1</v>
+      </c>
+      <c r="K101" s="2">
+        <v>1</v>
+      </c>
+      <c r="L101" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
         <v>97</v>
       </c>
       <c r="B102" s="2" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C102" s="2">
+        <v>12</v>
+      </c>
+      <c r="D102" s="2">
+        <v>45</v>
+      </c>
+      <c r="E102" s="2">
+        <v>48</v>
+      </c>
+      <c r="F102" s="2">
+        <v>49</v>
+      </c>
+      <c r="G102" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="H102" s="2">
+        <v>17</v>
+      </c>
+      <c r="I102" s="2">
+        <v>20</v>
+      </c>
+      <c r="J102" s="2">
+        <v>1</v>
+      </c>
+      <c r="K102" s="2">
+        <v>4</v>
+      </c>
+      <c r="L102" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
         <v>98</v>
       </c>
       <c r="B103" s="2" t="s">
         <v>146</v>
       </c>
+      <c r="C103" s="2">
+        <v>6</v>
+      </c>
+      <c r="D103" s="2">
+        <v>30</v>
+      </c>
       <c r="E103" s="2">
         <v>27</v>
       </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F103" s="2">
+        <v>72</v>
+      </c>
+      <c r="G103" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="H103" s="2">
+        <v>17</v>
+      </c>
+      <c r="I103" s="2">
+        <v>22</v>
+      </c>
+      <c r="J103" s="2">
+        <v>1</v>
+      </c>
+      <c r="K103" s="2">
+        <v>1</v>
+      </c>
+      <c r="L103" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
         <v>99</v>
       </c>
       <c r="B104" s="2" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C104" s="2">
+        <v>10</v>
+      </c>
+      <c r="D104" s="2">
+        <v>73</v>
+      </c>
+      <c r="E104" s="2">
+        <v>48</v>
+      </c>
+      <c r="F104" s="2">
+        <v>49</v>
+      </c>
+      <c r="G104" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="H104" s="2">
+        <v>17</v>
+      </c>
+      <c r="I104" s="2">
+        <v>20</v>
+      </c>
+      <c r="J104" s="2">
+        <v>1</v>
+      </c>
+      <c r="K104" s="2">
+        <v>4</v>
+      </c>
+      <c r="L104" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
         <v>100</v>
       </c>
       <c r="B105" s="2" t="s">
         <v>146</v>
       </c>
+      <c r="C105" s="2">
+        <v>6</v>
+      </c>
+      <c r="D105" s="2">
+        <v>30</v>
+      </c>
       <c r="E105" s="2">
         <v>27</v>
       </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F105" s="2">
+        <v>33</v>
+      </c>
+      <c r="G105" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="H105" s="2">
+        <v>17</v>
+      </c>
+      <c r="I105" s="2">
+        <v>22</v>
+      </c>
+      <c r="J105" s="2">
+        <v>1</v>
+      </c>
+      <c r="K105" s="2">
+        <v>1</v>
+      </c>
+      <c r="L105" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
         <v>101</v>
       </c>
       <c r="B106" s="2" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C106" s="2">
+        <v>12</v>
+      </c>
+      <c r="D106" s="2">
+        <v>45</v>
+      </c>
+      <c r="E106" s="2">
+        <v>51</v>
+      </c>
+      <c r="F106" s="2">
+        <v>50</v>
+      </c>
+      <c r="G106" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="H106" s="2">
+        <v>70</v>
+      </c>
+      <c r="I106" s="2">
+        <v>38</v>
+      </c>
+      <c r="J106" s="2">
+        <v>1</v>
+      </c>
+      <c r="K106" s="2">
+        <v>4</v>
+      </c>
+      <c r="L106" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
         <v>102</v>
       </c>
       <c r="B107" s="2" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C107" s="2">
+        <v>10</v>
+      </c>
+      <c r="D107" s="2">
+        <v>44</v>
+      </c>
+      <c r="E107" s="2">
+        <v>48</v>
+      </c>
+      <c r="F107" s="2">
+        <v>49</v>
+      </c>
+      <c r="G107" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="H107" s="2">
+        <v>17</v>
+      </c>
+      <c r="I107" s="2">
+        <v>20</v>
+      </c>
+      <c r="J107" s="2">
+        <v>1</v>
+      </c>
+      <c r="K107" s="2">
+        <v>4</v>
+      </c>
+      <c r="L107" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
         <v>103</v>
       </c>
       <c r="B108" s="2" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C108" s="2">
+        <v>2</v>
+      </c>
+      <c r="D108" s="2">
+        <v>17</v>
+      </c>
+      <c r="E108" s="2">
+        <v>21</v>
+      </c>
+      <c r="F108" s="2">
+        <v>22</v>
+      </c>
+      <c r="G108" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="H108" s="2">
+        <v>55</v>
+      </c>
+      <c r="I108" s="2">
+        <v>53</v>
+      </c>
+      <c r="J108" s="2">
+        <v>2</v>
+      </c>
+      <c r="K108" s="2">
+        <v>1</v>
+      </c>
+      <c r="L108" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
         <v>104</v>
       </c>
       <c r="B109" s="2" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C109" s="2">
+        <v>69</v>
+      </c>
+      <c r="D109" s="2">
+        <v>17</v>
+      </c>
+      <c r="E109" s="2">
+        <v>20</v>
+      </c>
+      <c r="F109" s="2">
+        <v>22</v>
+      </c>
+      <c r="G109" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="H109" s="2">
+        <v>66</v>
+      </c>
+      <c r="I109" s="2">
+        <v>50</v>
+      </c>
+      <c r="J109" s="2">
+        <v>2</v>
+      </c>
+      <c r="K109" s="2">
+        <v>4</v>
+      </c>
+      <c r="L109" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
         <v>105</v>
       </c>
       <c r="B110" s="2" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C110" s="2">
+        <v>7</v>
+      </c>
+      <c r="D110" s="2">
+        <v>35</v>
+      </c>
+      <c r="E110" s="2">
+        <v>37</v>
+      </c>
+      <c r="F110" s="2">
+        <v>40</v>
+      </c>
+      <c r="G110" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="H110" s="2">
+        <v>18</v>
+      </c>
+      <c r="I110" s="2">
+        <v>22</v>
+      </c>
+      <c r="J110" s="2">
+        <v>1</v>
+      </c>
+      <c r="K110" s="2">
+        <v>1</v>
+      </c>
+      <c r="L110" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
         <v>106</v>
       </c>
       <c r="B111" s="2" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C111" s="2">
+        <v>7</v>
+      </c>
+      <c r="D111" s="2">
+        <v>35</v>
+      </c>
+      <c r="E111" s="2">
+        <v>37</v>
+      </c>
+      <c r="F111" s="2">
+        <v>40</v>
+      </c>
+      <c r="G111" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="H111" s="2">
+        <v>18</v>
+      </c>
+      <c r="I111" s="2">
+        <v>22</v>
+      </c>
+      <c r="J111" s="2">
+        <v>1</v>
+      </c>
+      <c r="K111" s="2">
+        <v>1</v>
+      </c>
+      <c r="L111" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
         <v>107</v>
       </c>
       <c r="B112" s="2" t="s">
         <v>146</v>
       </c>
+      <c r="C112" s="2">
+        <v>4</v>
+      </c>
+      <c r="D112" s="2">
+        <v>28</v>
+      </c>
       <c r="E112" s="2">
         <v>27</v>
       </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F112" s="2">
+        <v>31</v>
+      </c>
+      <c r="G112" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="H112" s="2">
+        <v>17</v>
+      </c>
+      <c r="I112" s="2">
+        <v>22</v>
+      </c>
+      <c r="J112" s="2">
+        <v>1</v>
+      </c>
+      <c r="K112" s="2">
+        <v>4</v>
+      </c>
+      <c r="L112" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
         <v>108</v>
       </c>
       <c r="B113" s="2" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C113" s="2">
+        <v>12</v>
+      </c>
+      <c r="D113" s="2">
+        <v>73</v>
+      </c>
+      <c r="E113" s="2">
+        <v>66</v>
+      </c>
+      <c r="F113" s="2">
+        <v>50</v>
+      </c>
+      <c r="G113" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="H113" s="2">
+        <v>30</v>
+      </c>
+      <c r="I113" s="2">
+        <v>31</v>
+      </c>
+      <c r="J113" s="2">
+        <v>1</v>
+      </c>
+      <c r="K113" s="2">
+        <v>1</v>
+      </c>
+      <c r="L113" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
         <v>109</v>
       </c>
       <c r="B114" s="2" t="s">
         <v>146</v>
       </c>
+      <c r="C114" s="2">
+        <v>6</v>
+      </c>
+      <c r="D114" s="2">
+        <v>28</v>
+      </c>
       <c r="E114" s="2">
         <v>27</v>
       </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F114" s="2">
+        <v>72</v>
+      </c>
+      <c r="G114" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="H114" s="2">
+        <v>17</v>
+      </c>
+      <c r="I114" s="2">
+        <v>22</v>
+      </c>
+      <c r="J114" s="2">
+        <v>1</v>
+      </c>
+      <c r="K114" s="2">
+        <v>1</v>
+      </c>
+      <c r="L114" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
         <v>110</v>
       </c>
       <c r="B115" s="2" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C115" s="2">
+        <v>10</v>
+      </c>
+      <c r="D115" s="2">
+        <v>45</v>
+      </c>
+      <c r="E115" s="2">
+        <v>48</v>
+      </c>
+      <c r="F115" s="2">
+        <v>49</v>
+      </c>
+      <c r="G115" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="H115" s="2">
+        <v>17</v>
+      </c>
+      <c r="I115" s="2">
+        <v>20</v>
+      </c>
+      <c r="J115" s="2">
+        <v>2</v>
+      </c>
+      <c r="K115" s="2">
+        <v>4</v>
+      </c>
+      <c r="L115" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
         <v>111</v>
       </c>
       <c r="B116" s="2" t="s">
         <v>146</v>
       </c>
+      <c r="C116" s="2">
+        <v>6</v>
+      </c>
+      <c r="D116" s="2">
+        <v>28</v>
+      </c>
       <c r="E116" s="2">
         <v>27</v>
       </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F116" s="2">
+        <v>31</v>
+      </c>
+      <c r="G116" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="H116" s="2">
+        <v>17</v>
+      </c>
+      <c r="I116" s="2">
+        <v>22</v>
+      </c>
+      <c r="J116" s="2">
+        <v>1</v>
+      </c>
+      <c r="K116" s="2">
+        <v>1</v>
+      </c>
+      <c r="L116" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
         <v>112</v>
       </c>
       <c r="B117" s="2" t="s">
         <v>146</v>
       </c>
+      <c r="C117" s="2">
+        <v>6</v>
+      </c>
+      <c r="D117" s="2">
+        <v>30</v>
+      </c>
       <c r="E117" s="2">
         <v>27</v>
       </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F117" s="2">
+        <v>31</v>
+      </c>
+      <c r="G117" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="H117" s="2">
+        <v>17</v>
+      </c>
+      <c r="I117" s="2">
+        <v>22</v>
+      </c>
+      <c r="J117" s="2">
+        <v>1</v>
+      </c>
+      <c r="K117" s="2">
+        <v>1</v>
+      </c>
+      <c r="L117" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
         <v>113</v>
       </c>
       <c r="B118" s="2" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C118" s="2">
+        <v>12</v>
+      </c>
+      <c r="D118" s="2">
+        <v>45</v>
+      </c>
+      <c r="E118" s="2">
+        <v>48</v>
+      </c>
+      <c r="F118" s="2">
+        <v>50</v>
+      </c>
+      <c r="G118" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="H118" s="2">
+        <v>18</v>
+      </c>
+      <c r="I118" s="2">
+        <v>20</v>
+      </c>
+      <c r="J118" s="2">
+        <v>3</v>
+      </c>
+      <c r="K118" s="2">
+        <v>4</v>
+      </c>
+      <c r="L118" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
         <v>114</v>
       </c>
       <c r="B119" s="2" t="s">
         <v>146</v>
       </c>
+      <c r="C119" s="2">
+        <v>6</v>
+      </c>
+      <c r="D119" s="2">
+        <v>29</v>
+      </c>
       <c r="E119" s="2">
         <v>27</v>
       </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F119" s="2">
+        <v>31</v>
+      </c>
+      <c r="G119" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="H119" s="2">
+        <v>17</v>
+      </c>
+      <c r="I119" s="2">
+        <v>22</v>
+      </c>
+      <c r="J119" s="2">
+        <v>1</v>
+      </c>
+      <c r="K119" s="2">
+        <v>1</v>
+      </c>
+      <c r="L119" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
         <v>115</v>
       </c>
       <c r="B120" s="2" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C120" s="2">
+        <v>12</v>
+      </c>
+      <c r="D120" s="2">
+        <v>45</v>
+      </c>
+      <c r="E120" s="2">
+        <v>48</v>
+      </c>
+      <c r="F120" s="2">
+        <v>49</v>
+      </c>
+      <c r="G120" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="H120" s="2">
+        <v>17</v>
+      </c>
+      <c r="I120" s="2">
+        <v>20</v>
+      </c>
+      <c r="J120" s="2">
+        <v>3</v>
+      </c>
+      <c r="K120" s="2">
+        <v>4</v>
+      </c>
+      <c r="L120" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
         <v>116</v>
       </c>
       <c r="B121" s="2" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C121" s="2">
+        <v>1</v>
+      </c>
+      <c r="D121" s="2">
+        <v>17</v>
+      </c>
+      <c r="E121" s="2">
+        <v>21</v>
+      </c>
+      <c r="F121" s="2">
+        <v>22</v>
+      </c>
+      <c r="G121" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="H121" s="2">
+        <v>55</v>
+      </c>
+      <c r="I121" s="2">
+        <v>53</v>
+      </c>
+      <c r="J121" s="2">
+        <v>2</v>
+      </c>
+      <c r="K121" s="2">
+        <v>1</v>
+      </c>
+      <c r="L121" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
         <v>117</v>
       </c>
       <c r="B122" s="2" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C122" s="2">
+        <v>10</v>
+      </c>
+      <c r="D122" s="2">
+        <v>45</v>
+      </c>
+      <c r="E122" s="2">
+        <v>48</v>
+      </c>
+      <c r="F122" s="2">
+        <v>50</v>
+      </c>
+      <c r="G122" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="H122" s="2">
+        <v>17</v>
+      </c>
+      <c r="I122" s="2">
+        <v>20</v>
+      </c>
+      <c r="J122" s="2">
+        <v>2</v>
+      </c>
+      <c r="K122" s="2">
+        <v>4</v>
+      </c>
+      <c r="L122" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
         <v>118</v>
       </c>
       <c r="B123" s="2" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C123" s="2">
+        <v>2</v>
+      </c>
+      <c r="D123" s="2">
+        <v>17</v>
+      </c>
+      <c r="E123" s="2">
+        <v>21</v>
+      </c>
+      <c r="F123" s="2">
+        <v>24</v>
+      </c>
+      <c r="G123" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="H123" s="2">
+        <v>30</v>
+      </c>
+      <c r="I123" s="2">
+        <v>31</v>
+      </c>
+      <c r="J123" s="2">
+        <v>2</v>
+      </c>
+      <c r="K123" s="2">
+        <v>1</v>
+      </c>
+      <c r="L123" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
         <v>119</v>
       </c>
       <c r="B124" s="2" t="s">
         <v>146</v>
       </c>
+      <c r="C124" s="2">
+        <v>6</v>
+      </c>
+      <c r="D124" s="2">
+        <v>28</v>
+      </c>
       <c r="E124" s="2">
         <v>27</v>
       </c>
-    </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F124" s="2">
+        <v>31</v>
+      </c>
+      <c r="G124" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="H124" s="2">
+        <v>18</v>
+      </c>
+      <c r="I124" s="2">
+        <v>22</v>
+      </c>
+      <c r="J124" s="2">
+        <v>1</v>
+      </c>
+      <c r="K124" s="2">
+        <v>1</v>
+      </c>
+      <c r="L124" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
         <v>120</v>
       </c>
       <c r="B125" s="2" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C125" s="2">
+        <v>2</v>
+      </c>
+      <c r="D125" s="2">
+        <v>17</v>
+      </c>
+      <c r="E125" s="2">
+        <v>21</v>
+      </c>
+      <c r="F125" s="2">
+        <v>22</v>
+      </c>
+      <c r="G125" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="H125" s="2">
+        <v>30</v>
+      </c>
+      <c r="I125" s="2">
+        <v>72</v>
+      </c>
+      <c r="J125" s="2">
+        <v>2</v>
+      </c>
+      <c r="K125" s="2">
+        <v>1</v>
+      </c>
+      <c r="L125" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
         <v>121</v>
       </c>
       <c r="B126" s="2" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C126" s="2">
+        <v>69</v>
+      </c>
+      <c r="D126" s="2">
+        <v>17</v>
+      </c>
+      <c r="E126" s="2">
+        <v>20</v>
+      </c>
+      <c r="F126" s="2">
+        <v>22</v>
+      </c>
+      <c r="G126" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="H126" s="2">
+        <v>50</v>
+      </c>
+      <c r="I126" s="2">
+        <v>66</v>
+      </c>
+      <c r="J126" s="2">
+        <v>2</v>
+      </c>
+      <c r="K126" s="2">
+        <v>4</v>
+      </c>
+      <c r="L126" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
         <v>122</v>
       </c>
       <c r="B127" s="2" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C127" s="2">
+        <v>69</v>
+      </c>
+      <c r="D127" s="2">
+        <v>17</v>
+      </c>
+      <c r="E127" s="2">
+        <v>20</v>
+      </c>
+      <c r="F127" s="2">
+        <v>24</v>
+      </c>
+      <c r="G127" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="H127" s="2">
+        <v>50</v>
+      </c>
+      <c r="I127" s="2">
+        <v>66</v>
+      </c>
+      <c r="J127" s="2">
+        <v>1</v>
+      </c>
+      <c r="K127" s="2">
+        <v>4</v>
+      </c>
+      <c r="L127" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="B128" s="2" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C128" s="2">
+        <v>2</v>
+      </c>
+      <c r="D128" s="2">
+        <v>17</v>
+      </c>
+      <c r="E128" s="2">
+        <v>21</v>
+      </c>
+      <c r="F128" s="2">
+        <v>22</v>
+      </c>
+      <c r="G128" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="H128" s="2">
+        <v>55</v>
+      </c>
+      <c r="I128" s="2">
+        <v>53</v>
+      </c>
+      <c r="J128" s="2">
+        <v>2</v>
+      </c>
+      <c r="K128" s="2">
+        <v>1</v>
+      </c>
+      <c r="L128" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="129" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="B129" s="2" t="s">
         <v>146</v>
       </c>
+      <c r="C129" s="2">
+        <v>6</v>
+      </c>
+      <c r="D129" s="2">
+        <v>29</v>
+      </c>
       <c r="E129" s="2">
         <v>27</v>
       </c>
-    </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F129" s="2">
+        <v>31</v>
+      </c>
+      <c r="G129" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="H129" s="2">
+        <v>17</v>
+      </c>
+      <c r="I129" s="2">
+        <v>22</v>
+      </c>
+      <c r="J129" s="2">
+        <v>1</v>
+      </c>
+      <c r="K129" s="2">
+        <v>1</v>
+      </c>
+      <c r="L129" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="130" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
         <v>123</v>
       </c>
       <c r="B130" s="2" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C130" s="2">
+        <v>3</v>
+      </c>
+      <c r="D130" s="2">
+        <v>17</v>
+      </c>
+      <c r="E130" s="2">
+        <v>19</v>
+      </c>
+      <c r="F130" s="2">
+        <v>22</v>
+      </c>
+      <c r="G130" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="H130" s="2">
+        <v>55</v>
+      </c>
+      <c r="I130" s="2">
+        <v>53</v>
+      </c>
+      <c r="J130" s="2">
+        <v>2</v>
+      </c>
+      <c r="K130" s="2">
+        <v>1</v>
+      </c>
+      <c r="L130" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="131" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
         <v>124</v>
       </c>
       <c r="B131" s="2" t="s">
         <v>146</v>
       </c>
+      <c r="C131" s="2">
+        <v>6</v>
+      </c>
+      <c r="D131" s="2">
+        <v>28</v>
+      </c>
       <c r="E131" s="2">
         <v>27</v>
       </c>
-    </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F131" s="2">
+        <v>72</v>
+      </c>
+      <c r="G131" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="H131" s="2">
+        <v>18</v>
+      </c>
+      <c r="I131" s="2">
+        <v>22</v>
+      </c>
+      <c r="J131" s="2">
+        <v>1</v>
+      </c>
+      <c r="K131" s="2">
+        <v>1</v>
+      </c>
+      <c r="L131" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="132" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
         <v>125</v>
       </c>
       <c r="B132" s="2" t="s">
         <v>146</v>
       </c>
+      <c r="C132" s="2">
+        <v>6</v>
+      </c>
+      <c r="D132" s="2">
+        <v>28</v>
+      </c>
       <c r="E132" s="2">
         <v>27</v>
       </c>
-    </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F132" s="2">
+        <v>72</v>
+      </c>
+      <c r="G132" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="H132" s="2">
+        <v>18</v>
+      </c>
+      <c r="I132" s="2">
+        <v>22</v>
+      </c>
+      <c r="J132" s="2">
+        <v>1</v>
+      </c>
+      <c r="K132" s="2">
+        <v>1</v>
+      </c>
+      <c r="L132" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="133" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
         <v>126</v>
       </c>
       <c r="B133" s="2" t="s">
         <v>146</v>
       </c>
+      <c r="C133" s="2">
+        <v>71</v>
+      </c>
+      <c r="D133" s="2">
+        <v>30</v>
+      </c>
       <c r="E133" s="2">
         <v>27</v>
       </c>
-    </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F133" s="2">
+        <v>72</v>
+      </c>
+      <c r="G133" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="H133" s="2">
+        <v>17</v>
+      </c>
+      <c r="I133" s="2">
+        <v>22</v>
+      </c>
+      <c r="J133" s="2">
+        <v>1</v>
+      </c>
+      <c r="K133" s="2">
+        <v>1</v>
+      </c>
+      <c r="L133" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="134" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
         <v>127</v>
       </c>
       <c r="B134" s="2" t="s">
         <v>146</v>
       </c>
+      <c r="C134" s="2">
+        <v>6</v>
+      </c>
+      <c r="D134" s="2">
+        <v>29</v>
+      </c>
       <c r="E134" s="2">
         <v>27</v>
       </c>
-    </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F134" s="2">
+        <v>31</v>
+      </c>
+      <c r="G134" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="H134" s="2">
+        <v>18</v>
+      </c>
+      <c r="I134" s="2">
+        <v>22</v>
+      </c>
+      <c r="J134" s="2">
+        <v>1</v>
+      </c>
+      <c r="K134" s="2">
+        <v>1</v>
+      </c>
+      <c r="L134" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="135" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
         <v>128</v>
       </c>
       <c r="B135" s="2" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C135" s="2">
+        <v>9</v>
+      </c>
+      <c r="D135" s="2">
+        <v>70</v>
+      </c>
+      <c r="E135" s="2">
+        <v>38</v>
+      </c>
+      <c r="F135" s="2">
+        <v>40</v>
+      </c>
+      <c r="G135" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="H135" s="2">
+        <v>17</v>
+      </c>
+      <c r="I135" s="2">
+        <v>22</v>
+      </c>
+      <c r="J135" s="2">
+        <v>1</v>
+      </c>
+      <c r="K135" s="2">
+        <v>1</v>
+      </c>
+      <c r="L135" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="136" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
         <v>129</v>
       </c>
       <c r="B136" s="2" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C136" s="2">
+        <v>10</v>
+      </c>
+      <c r="D136" s="2">
+        <v>45</v>
+      </c>
+      <c r="E136" s="2">
+        <v>48</v>
+      </c>
+      <c r="F136" s="2">
+        <v>49</v>
+      </c>
+      <c r="G136" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="H136" s="2">
+        <v>17</v>
+      </c>
+      <c r="I136" s="2">
+        <v>20</v>
+      </c>
+      <c r="J136" s="2">
+        <v>2</v>
+      </c>
+      <c r="K136" s="2">
+        <v>4</v>
+      </c>
+      <c r="L136" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="137" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
         <v>130</v>
       </c>
       <c r="B137" s="2" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C137" s="2">
+        <v>10</v>
+      </c>
+      <c r="D137" s="2">
+        <v>45</v>
+      </c>
+      <c r="E137" s="2">
+        <v>48</v>
+      </c>
+      <c r="F137" s="2">
+        <v>49</v>
+      </c>
+      <c r="G137" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="H137" s="2">
+        <v>17</v>
+      </c>
+      <c r="I137" s="2">
+        <v>20</v>
+      </c>
+      <c r="J137" s="2">
+        <v>2</v>
+      </c>
+      <c r="K137" s="2">
+        <v>4</v>
+      </c>
+      <c r="L137" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="138" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
         <v>131</v>
       </c>
       <c r="B138" s="2" t="s">
         <v>146</v>
       </c>
+      <c r="C138" s="2">
+        <v>6</v>
+      </c>
+      <c r="D138" s="2">
+        <v>30</v>
+      </c>
       <c r="E138" s="2">
         <v>27</v>
       </c>
-    </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F138" s="2">
+        <v>72</v>
+      </c>
+      <c r="G138" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="H138" s="2">
+        <v>17</v>
+      </c>
+      <c r="I138" s="2">
+        <v>22</v>
+      </c>
+      <c r="J138" s="2">
+        <v>1</v>
+      </c>
+      <c r="K138" s="2">
+        <v>1</v>
+      </c>
+      <c r="L138" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="139" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
         <v>132</v>
       </c>
       <c r="B139" s="2" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C139" s="2">
+        <v>2</v>
+      </c>
+      <c r="D139" s="2">
+        <v>17</v>
+      </c>
+      <c r="E139" s="2">
+        <v>21</v>
+      </c>
+      <c r="F139" s="2">
+        <v>22</v>
+      </c>
+      <c r="G139" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="H139" s="2">
+        <v>55</v>
+      </c>
+      <c r="I139" s="2">
+        <v>53</v>
+      </c>
+      <c r="J139" s="2">
+        <v>2</v>
+      </c>
+      <c r="K139" s="2">
+        <v>1</v>
+      </c>
+      <c r="L139" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="140" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
         <v>133</v>
       </c>
       <c r="B140" s="2" t="s">
         <v>146</v>
       </c>
+      <c r="C140" s="2">
+        <v>6</v>
+      </c>
+      <c r="D140" s="2">
+        <v>29</v>
+      </c>
       <c r="E140" s="2">
         <v>27</v>
       </c>
-    </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F140" s="2">
+        <v>72</v>
+      </c>
+      <c r="G140" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="H140" s="2">
+        <v>17</v>
+      </c>
+      <c r="I140" s="2">
+        <v>22</v>
+      </c>
+      <c r="J140" s="2">
+        <v>1</v>
+      </c>
+      <c r="K140" s="2">
+        <v>1</v>
+      </c>
+      <c r="L140" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="141" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
         <v>134</v>
       </c>
       <c r="B141" s="2" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C141" s="2">
+        <v>69</v>
+      </c>
+      <c r="D141" s="2">
+        <v>17</v>
+      </c>
+      <c r="E141" s="2">
+        <v>20</v>
+      </c>
+      <c r="F141" s="2">
+        <v>22</v>
+      </c>
+      <c r="G141" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="H141" s="2">
+        <v>50</v>
+      </c>
+      <c r="I141" s="2">
+        <v>66</v>
+      </c>
+      <c r="J141" s="2">
+        <v>2</v>
+      </c>
+      <c r="K141" s="2">
+        <v>1</v>
+      </c>
+      <c r="L141" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="142" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
         <v>135</v>
       </c>
       <c r="B142" s="2" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C142" s="2">
+        <v>69</v>
+      </c>
+      <c r="D142" s="2">
+        <v>17</v>
+      </c>
+      <c r="E142" s="2">
+        <v>19</v>
+      </c>
+      <c r="F142" s="2">
+        <v>22</v>
+      </c>
+      <c r="G142" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="H142" s="2">
+        <v>30</v>
+      </c>
+      <c r="I142" s="2">
+        <v>31</v>
+      </c>
+      <c r="J142" s="2">
+        <v>2</v>
+      </c>
+      <c r="K142" s="2">
+        <v>1</v>
+      </c>
+      <c r="L142" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="143" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
         <v>136</v>
       </c>
       <c r="B143" s="2" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C143" s="2">
+        <v>10</v>
+      </c>
+      <c r="D143" s="2">
+        <v>44</v>
+      </c>
+      <c r="E143" s="2">
+        <v>66</v>
+      </c>
+      <c r="F143" s="2">
+        <v>49</v>
+      </c>
+      <c r="G143" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="H143" s="2">
+        <v>17</v>
+      </c>
+      <c r="I143" s="2">
+        <v>20</v>
+      </c>
+      <c r="J143" s="2">
+        <v>2</v>
+      </c>
+      <c r="K143" s="2">
+        <v>4</v>
+      </c>
+      <c r="L143" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="144" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
         <v>137</v>
       </c>
       <c r="B144" s="2" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C144" s="2">
+        <v>7</v>
+      </c>
+      <c r="D144" s="2">
+        <v>35</v>
+      </c>
+      <c r="E144" s="2">
+        <v>37</v>
+      </c>
+      <c r="F144" s="2">
+        <v>40</v>
+      </c>
+      <c r="G144" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="H144" s="2">
+        <v>18</v>
+      </c>
+      <c r="I144" s="2">
+        <v>22</v>
+      </c>
+      <c r="J144" s="2">
+        <v>1</v>
+      </c>
+      <c r="K144" s="2">
+        <v>1</v>
+      </c>
+      <c r="L144" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="145" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
         <v>138</v>
       </c>
       <c r="B145" s="2" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C145" s="2">
+        <v>12</v>
+      </c>
+      <c r="D145" s="2">
+        <v>45</v>
+      </c>
+      <c r="E145" s="2">
+        <v>48</v>
+      </c>
+      <c r="F145" s="2">
+        <v>49</v>
+      </c>
+      <c r="G145" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="H145" s="2">
+        <v>17</v>
+      </c>
+      <c r="I145" s="2">
+        <v>20</v>
+      </c>
+      <c r="J145" s="2">
+        <v>1</v>
+      </c>
+      <c r="K145" s="2">
+        <v>4</v>
+      </c>
+      <c r="L145" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="146" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
         <v>139</v>
       </c>
       <c r="B146" s="2" t="s">
         <v>146</v>
       </c>
+      <c r="C146" s="2">
+        <v>6</v>
+      </c>
+      <c r="D146" s="2">
+        <v>30</v>
+      </c>
       <c r="E146" s="2">
         <v>27</v>
       </c>
-    </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F146" s="2">
+        <v>31</v>
+      </c>
+      <c r="G146" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="H146" s="2">
+        <v>17</v>
+      </c>
+      <c r="I146" s="2">
+        <v>22</v>
+      </c>
+      <c r="J146" s="2">
+        <v>1</v>
+      </c>
+      <c r="K146" s="2">
+        <v>1</v>
+      </c>
+      <c r="L146" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="147" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
         <v>140</v>
       </c>
       <c r="B147" s="2" t="s">
         <v>146</v>
       </c>
+      <c r="C147" s="2">
+        <v>6</v>
+      </c>
+      <c r="D147" s="2">
+        <v>29</v>
+      </c>
       <c r="E147" s="2">
         <v>27</v>
       </c>
-    </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F147" s="2">
+        <v>72</v>
+      </c>
+      <c r="G147" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="H147" s="2">
+        <v>18</v>
+      </c>
+      <c r="I147" s="2">
+        <v>22</v>
+      </c>
+      <c r="J147" s="2">
+        <v>1</v>
+      </c>
+      <c r="K147" s="2">
+        <v>1</v>
+      </c>
+      <c r="L147" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="148" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
         <v>141</v>
       </c>
       <c r="B148" s="2" t="s">
         <v>146</v>
       </c>
+      <c r="C148" s="2">
+        <v>4</v>
+      </c>
+      <c r="D148" s="2">
+        <v>29</v>
+      </c>
       <c r="E148" s="2">
         <v>27</v>
       </c>
-    </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F148" s="2">
+        <v>72</v>
+      </c>
+      <c r="G148" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="H148" s="2">
+        <v>18</v>
+      </c>
+      <c r="I148" s="2">
+        <v>22</v>
+      </c>
+      <c r="J148" s="2">
+        <v>1</v>
+      </c>
+      <c r="K148" s="2">
+        <v>1</v>
+      </c>
+      <c r="L148" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="149" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
         <v>142</v>
       </c>
       <c r="B149" s="2" t="s">
         <v>146</v>
       </c>
+      <c r="C149" s="2">
+        <v>6</v>
+      </c>
+      <c r="D149" s="2">
+        <v>30</v>
+      </c>
       <c r="E149" s="2">
         <v>27</v>
       </c>
-    </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F149" s="2">
+        <v>33</v>
+      </c>
+      <c r="G149" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="H149" s="2">
+        <v>17</v>
+      </c>
+      <c r="I149" s="2">
+        <v>22</v>
+      </c>
+      <c r="J149" s="2">
+        <v>1</v>
+      </c>
+      <c r="K149" s="2">
+        <v>1</v>
+      </c>
+      <c r="L149" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="150" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
         <v>143</v>
       </c>
       <c r="B150" s="2" t="s">
         <v>146</v>
       </c>
+      <c r="C150" s="2">
+        <v>6</v>
+      </c>
+      <c r="D150" s="2">
+        <v>29</v>
+      </c>
       <c r="E150" s="2">
         <v>27</v>
+      </c>
+      <c r="F150" s="2">
+        <v>72</v>
+      </c>
+      <c r="G150" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="H150" s="2">
+        <v>18</v>
+      </c>
+      <c r="I150" s="2">
+        <v>22</v>
+      </c>
+      <c r="J150" s="2">
+        <v>1</v>
+      </c>
+      <c r="K150" s="2">
+        <v>1</v>
+      </c>
+      <c r="L150" s="2">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>